<commit_message>
Performed timescale analysis, updated control experiments, ran polydisperse experiments, wrote up small conclusions in jupyter notebooks
</commit_message>
<xml_diff>
--- a/calculations/04172018_tRNAModelCalculations.xlsx
+++ b/calculations/04172018_tRNAModelCalculations.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>sub-vol=</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>sub-vol (1/1621)</t>
+  </si>
+  <si>
+    <t>1 tRNA extimate</t>
   </si>
 </sst>
 </file>
@@ -149,8 +152,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -181,7 +188,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -191,6 +198,8 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -200,6 +209,8 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -529,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:M18"/>
+  <dimension ref="A3:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -540,7 +551,7 @@
     <col min="7" max="7" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:13" ht="90">
+    <row r="3" spans="1:17" ht="90">
       <c r="A3" s="4" t="s">
         <v>15</v>
       </c>
@@ -565,7 +576,7 @@
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:17">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -596,7 +607,7 @@
         <v>27.410826392204708</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:17">
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
@@ -624,7 +635,7 @@
         <v>43.857322227527533</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:17">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -652,7 +663,7 @@
         <v>131.5719666825826</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:17">
       <c r="B7" s="2"/>
       <c r="C7">
         <v>64000</v>
@@ -664,7 +675,7 @@
         <v>39.481801357186924</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:17">
       <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
@@ -692,7 +703,7 @@
         <v>1061.0642474401825</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:17">
       <c r="B9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2">
@@ -700,48 +711,169 @@
         <v>0.21992580453742464</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
-      <c r="H11" t="s">
+    <row r="11" spans="1:17">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>12</v>
+      </c>
+      <c r="E11" s="2">
+        <f>(4/3)*3.1415*(D11*0.001)^3</f>
+        <v>7.2380159999999996E-6</v>
+      </c>
+      <c r="F11" s="2">
+        <f>E11*C11</f>
+        <v>7.2380159999999996E-6</v>
+      </c>
+      <c r="G11">
+        <f>C11/1621</f>
+        <v>6.1690314620604567E-4</v>
+      </c>
+      <c r="H11">
+        <f>((1.38*10^-23*310)/(6*3.1415*(6.9*10^-4)*(D11*10^-9)))*10^12</f>
+        <v>27.410826392204708</v>
+      </c>
+      <c r="L11" t="s">
         <v>0</v>
       </c>
-      <c r="I11">
+      <c r="M11">
         <f>C5/47</f>
         <v>1621.0739614994936</v>
       </c>
-      <c r="M11" t="s">
+      <c r="Q11" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:17">
+      <c r="B12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>7</v>
+      </c>
+      <c r="D12">
+        <v>7.5</v>
+      </c>
+      <c r="E12" s="2">
+        <f>(4/3)*3.1415*(D12*0.001)^3</f>
+        <v>1.7670937499999998E-6</v>
+      </c>
+      <c r="F12" s="2">
+        <f t="shared" ref="F12:F15" si="2">E12*C12</f>
+        <v>1.2369656249999998E-5</v>
+      </c>
+      <c r="G12">
+        <f t="shared" ref="G12:G15" si="3">C12/1621</f>
+        <v>4.3183220234423196E-3</v>
+      </c>
       <c r="H12">
-        <f>C4/I11</f>
+        <f>((1.38*10^-23*310)/(6*3.1415*(6.9*10^-4)*(D12*10^-9)))*10^12</f>
+        <v>43.857322227527533</v>
+      </c>
+      <c r="L12">
+        <f>C4/M11</f>
         <v>7.1781818181818169</v>
       </c>
-      <c r="I12" t="s">
+      <c r="M12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:17">
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>2.5</v>
+      </c>
+      <c r="E13" s="2">
+        <f>(4/3)*3.1415*(D13*0.001)^3</f>
+        <v>6.5447916666666669E-8</v>
+      </c>
+      <c r="F13" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="H13">
-        <f>C5/I11</f>
+        <f>((1.38*10^-23*310)/(6*3.1415*(6.9*10^-4)*(D13*10^-9)))*10^12</f>
+        <v>131.5719666825826</v>
+      </c>
+      <c r="L13">
+        <f>C5/M11</f>
         <v>47</v>
       </c>
-      <c r="I13" t="s">
+      <c r="M13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
-      <c r="H14">
-        <f>C6/I11</f>
+    <row r="14" spans="1:17">
+      <c r="B14" s="2"/>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <f>C6/M11</f>
         <v>8.3999999999999986</v>
       </c>
-      <c r="I14" t="s">
+      <c r="M14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
-      <c r="H16">
-        <f>C8/I11</f>
+    <row r="15" spans="1:17">
+      <c r="B15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0.31</v>
+      </c>
+      <c r="E15" s="2">
+        <f>(4/3)*3.1415*(D15*0.001)^3</f>
+        <v>1.2478456866666664E-10</v>
+      </c>
+      <c r="F15" s="2">
+        <f t="shared" ref="F15:F16" si="4">E15*C15</f>
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <f>((1.38*10^-23*310)/(6*3.1415*(6.9*10^-4)*(D15*10^-9)))*10^12</f>
+        <v>1061.0642474401825</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="B16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2">
+        <f>SUM(F11:F15)</f>
+        <v>1.9607672249999998E-5</v>
+      </c>
+      <c r="L16">
+        <f>C8/M11</f>
         <v>863.62499999999989</v>
       </c>
     </row>

</xml_diff>